<commit_message>
updating models and scripts
</commit_message>
<xml_diff>
--- a/data/2023_SAFE_biomass_estimate.xlsx
+++ b/data/2023_SAFE_biomass_estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant.adams\GitHub\GOA ATF ESP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D4F097-5B38-4992-9199-C528249D275A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9265BF56-98B7-417A-8152-76565B7F1CFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="885" yWindow="1455" windowWidth="24645" windowHeight="13380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>Year</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Recruitment</t>
+  </si>
+  <si>
+    <t>Catch</t>
   </si>
 </sst>
 </file>
@@ -2074,7 +2077,7 @@
   <dimension ref="A1:BB57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2092,6 +2095,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -2106,6 +2112,9 @@
       <c r="D2" s="3">
         <v>601013000</v>
       </c>
+      <c r="E2">
+        <v>9447.0400000000009</v>
+      </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -2119,6 +2128,9 @@
       </c>
       <c r="D3" s="3">
         <v>694993000</v>
+      </c>
+      <c r="E3">
+        <v>8407.9599999999991</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -2181,6 +2193,9 @@
       <c r="D4" s="3">
         <v>753141000</v>
       </c>
+      <c r="E4">
+        <v>7577.53</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -2242,6 +2257,9 @@
       <c r="D5" s="3">
         <v>682679000</v>
       </c>
+      <c r="E5">
+        <v>7846.2</v>
+      </c>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
@@ -2264,6 +2282,9 @@
       <c r="D6" s="3">
         <v>568624000</v>
       </c>
+      <c r="E6">
+        <v>7431.79</v>
+      </c>
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
@@ -2285,6 +2306,9 @@
       </c>
       <c r="D7" s="3">
         <v>551128000</v>
+      </c>
+      <c r="E7">
+        <v>4638.74</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2347,6 +2371,9 @@
       <c r="D8" s="3">
         <v>633613000</v>
       </c>
+      <c r="E8">
+        <v>6330.08</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -2408,6 +2435,9 @@
       <c r="D9" s="3">
         <v>868275000</v>
       </c>
+      <c r="E9">
+        <v>3456.04</v>
+      </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2422,6 +2452,9 @@
       <c r="D10" s="3">
         <v>1220710000</v>
       </c>
+      <c r="E10">
+        <v>1538.72</v>
+      </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2436,6 +2469,9 @@
       <c r="D11" s="3">
         <v>1065810000</v>
       </c>
+      <c r="E11">
+        <v>1220.8800000000001</v>
+      </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
@@ -2451,6 +2487,9 @@
       <c r="D12" s="3">
         <v>1007980000</v>
       </c>
+      <c r="E12">
+        <v>4962.34</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
@@ -2466,6 +2505,9 @@
       <c r="D13" s="3">
         <v>1088210000</v>
       </c>
+      <c r="E13">
+        <v>5137.38</v>
+      </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
@@ -2481,6 +2523,9 @@
       <c r="D14" s="3">
         <v>1029070000</v>
       </c>
+      <c r="E14">
+        <v>2583.5300000000002</v>
+      </c>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
@@ -2496,6 +2541,9 @@
       <c r="D15" s="3">
         <v>891503000</v>
       </c>
+      <c r="E15">
+        <v>7705.03</v>
+      </c>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
@@ -2511,6 +2559,9 @@
       <c r="D16" s="3">
         <v>964597000</v>
       </c>
+      <c r="E16">
+        <v>17385.7</v>
+      </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2526,6 +2577,9 @@
       <c r="D17" s="3">
         <v>941008000</v>
       </c>
+      <c r="E17">
+        <v>21912.1</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2541,6 +2595,9 @@
       <c r="D18" s="3">
         <v>719768000</v>
       </c>
+      <c r="E18">
+        <v>19074.900000000001</v>
+      </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2556,6 +2613,9 @@
       <c r="D19" s="3">
         <v>715897000</v>
       </c>
+      <c r="E19">
+        <v>22915.5</v>
+      </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2571,6 +2631,9 @@
       <c r="D20" s="3">
         <v>770326000</v>
       </c>
+      <c r="E20">
+        <v>18277.7</v>
+      </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2586,6 +2649,9 @@
       <c r="D21" s="3">
         <v>747329000</v>
       </c>
+      <c r="E21">
+        <v>22480.9</v>
+      </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2601,6 +2667,9 @@
       <c r="D22" s="3">
         <v>880412000</v>
       </c>
+      <c r="E22">
+        <v>16360.9</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2616,6 +2685,9 @@
       <c r="D23" s="3">
         <v>1108610000</v>
       </c>
+      <c r="E23">
+        <v>12956.4</v>
+      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2631,6 +2703,9 @@
       <c r="D24" s="3">
         <v>1202270000</v>
       </c>
+      <c r="E24">
+        <v>16141.9</v>
+      </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2646,6 +2721,9 @@
       <c r="D25" s="3">
         <v>1555480000</v>
       </c>
+      <c r="E25">
+        <v>24206.7</v>
+      </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2661,6 +2739,9 @@
       <c r="D26" s="3">
         <v>1032550000</v>
       </c>
+      <c r="E26">
+        <v>19924.900000000001</v>
+      </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2676,6 +2757,9 @@
       <c r="D27" s="3">
         <v>957785000</v>
       </c>
+      <c r="E27">
+        <v>21212.6</v>
+      </c>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2691,6 +2775,9 @@
       <c r="D28" s="3">
         <v>882391000</v>
       </c>
+      <c r="E28">
+        <v>30254.5</v>
+      </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2706,6 +2793,9 @@
       <c r="D29" s="3">
         <v>938885000</v>
       </c>
+      <c r="E29">
+        <v>15755.4</v>
+      </c>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2721,6 +2811,9 @@
       <c r="D30" s="3">
         <v>985795000</v>
       </c>
+      <c r="E30">
+        <v>19988</v>
+      </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2736,6 +2829,9 @@
       <c r="D31" s="3">
         <v>912955000</v>
       </c>
+      <c r="E31">
+        <v>27740</v>
+      </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2751,6 +2847,9 @@
       <c r="D32" s="3">
         <v>662066000</v>
       </c>
+      <c r="E32">
+        <v>25509.599999999999</v>
+      </c>
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2766,6 +2865,9 @@
       <c r="D33" s="3">
         <v>644075000</v>
       </c>
+      <c r="E33">
+        <v>29270</v>
+      </c>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2781,6 +2883,9 @@
       <c r="D34" s="3">
         <v>463970000</v>
       </c>
+      <c r="E34">
+        <v>24911.8</v>
+      </c>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2796,6 +2901,9 @@
       <c r="D35" s="3">
         <v>451717000</v>
       </c>
+      <c r="E35">
+        <v>24495.200000000001</v>
+      </c>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2811,6 +2919,9 @@
       <c r="D36" s="3">
         <v>600732000</v>
       </c>
+      <c r="E36">
+        <v>30965.9</v>
+      </c>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2826,6 +2937,9 @@
       <c r="D37" s="3">
         <v>744114000</v>
       </c>
+      <c r="E37">
+        <v>20620</v>
+      </c>
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2841,6 +2955,9 @@
       <c r="D38" s="3">
         <v>781273000</v>
       </c>
+      <c r="E38">
+        <v>21537.8</v>
+      </c>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2856,6 +2973,9 @@
       <c r="D39" s="3">
         <v>639415000</v>
       </c>
+      <c r="E39">
+        <v>36311</v>
+      </c>
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2871,6 +2991,9 @@
       <c r="D40" s="3">
         <v>550236000</v>
       </c>
+      <c r="E40">
+        <v>19084.900000000001</v>
+      </c>
       <c r="I40" s="3"/>
       <c r="K40" s="3"/>
     </row>
@@ -2887,6 +3010,9 @@
       <c r="D41" s="3">
         <v>633468000</v>
       </c>
+      <c r="E41">
+        <v>19819.8</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="K41" s="3"/>
     </row>
@@ -2903,6 +3029,9 @@
       <c r="D42" s="3">
         <v>684650000</v>
       </c>
+      <c r="E42">
+        <v>26902.400000000001</v>
+      </c>
       <c r="I42" s="3"/>
       <c r="K42" s="3"/>
     </row>
@@ -2919,6 +3048,9 @@
       <c r="D43" s="3">
         <v>974684000</v>
       </c>
+      <c r="E43">
+        <v>18833</v>
+      </c>
       <c r="I43" s="3"/>
       <c r="K43" s="3"/>
     </row>
@@ -2935,6 +3067,9 @@
       <c r="D44" s="3">
         <v>496959000</v>
       </c>
+      <c r="E44">
+        <v>24584.7</v>
+      </c>
       <c r="I44" s="3"/>
       <c r="K44" s="3"/>
     </row>
@@ -2951,6 +3086,9 @@
       <c r="D45" s="3">
         <v>643247000</v>
       </c>
+      <c r="E45">
+        <v>21125</v>
+      </c>
       <c r="I45" s="3"/>
       <c r="K45" s="3"/>
     </row>
@@ -2967,6 +3105,9 @@
       <c r="D46" s="3">
         <v>684898000</v>
       </c>
+      <c r="E46">
+        <v>9988.0300000000007</v>
+      </c>
       <c r="I46" s="3"/>
       <c r="K46" s="3"/>
     </row>
@@ -2983,6 +3124,9 @@
       <c r="D47" s="3">
         <v>713088000</v>
       </c>
+      <c r="E47">
+        <v>11630.1</v>
+      </c>
       <c r="I47" s="3"/>
       <c r="K47" s="3"/>
     </row>
@@ -2998,6 +3142,9 @@
       </c>
       <c r="D48" s="3">
         <v>436000000</v>
+      </c>
+      <c r="E48">
+        <v>9028.42</v>
       </c>
       <c r="I48" s="3"/>
     </row>

</xml_diff>

<commit_message>
update CEATTLE to ADMB
</commit_message>
<xml_diff>
--- a/data/2023_SAFE_biomass_estimate.xlsx
+++ b/data/2023_SAFE_biomass_estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\GOA-ATF-ESP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8169FAF0-2EEC-4EEF-B358-13A433A9153B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E884AC15-061F-419B-BAF4-FEEF4D51C0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2340" windowWidth="23775" windowHeight="12210" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="2505" windowWidth="23775" windowHeight="9645" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023 SAFE" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,21 @@
     <sheet name="2023 SAFE selectivity" sheetId="6" r:id="rId6"/>
     <sheet name="ADMB CEATTLE par" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1593,8 +1604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AT48"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16244,15 +16255,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDA3F8D-107B-435D-85B7-C62AB9736DED}">
-  <dimension ref="A1:BA48"/>
+  <dimension ref="A1:AZ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16266,710 +16280,733 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1977</v>
       </c>
       <c r="B2" s="1">
-        <v>1231640</v>
+        <v>1116280</v>
       </c>
       <c r="C2" s="1">
-        <v>732097</v>
+        <v>663629</v>
       </c>
       <c r="D2" s="1">
-        <v>600780000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+        <v>552082000</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1978</v>
       </c>
       <c r="B3" s="1">
-        <v>1221440</v>
+        <v>1109810</v>
       </c>
       <c r="C3" s="1">
-        <v>725700</v>
+        <v>654783</v>
       </c>
       <c r="D3" s="1">
-        <v>641720000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+        <v>629128000</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1979</v>
       </c>
       <c r="B4" s="1">
-        <v>1219300</v>
+        <v>1112900</v>
       </c>
       <c r="C4" s="1">
-        <v>717993</v>
+        <v>646473</v>
       </c>
       <c r="D4" s="1">
-        <v>706407000</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
-      <c r="AT4" s="1"/>
-      <c r="AU4" s="1"/>
-      <c r="AV4" s="1"/>
-      <c r="AW4" s="1"/>
-      <c r="AX4" s="1"/>
-      <c r="AY4" s="1"/>
-      <c r="AZ4" s="1"/>
-      <c r="BA4" s="1"/>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+        <v>704271000</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1980</v>
       </c>
       <c r="B5" s="1">
-        <v>1219120</v>
+        <v>1121110</v>
       </c>
       <c r="C5" s="1">
-        <v>709296</v>
+        <v>638330</v>
       </c>
       <c r="D5" s="1">
-        <v>625524000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+        <v>665921000</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1981</v>
       </c>
       <c r="B6" s="1">
-        <v>1215990</v>
+        <v>1127980</v>
       </c>
       <c r="C6" s="1">
-        <v>699284</v>
+        <v>629942</v>
       </c>
       <c r="D6" s="1">
-        <v>545618000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+        <v>574355000</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1982</v>
       </c>
       <c r="B7" s="1">
-        <v>1210410</v>
+        <v>1133300</v>
       </c>
       <c r="C7" s="1">
-        <v>690597</v>
+        <v>623465</v>
       </c>
       <c r="D7" s="1">
-        <v>523016000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+        <v>546572000</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1983</v>
       </c>
       <c r="B8" s="1">
-        <v>1208670</v>
+        <v>1142750</v>
       </c>
       <c r="C8" s="1">
-        <v>687868</v>
+        <v>623287</v>
       </c>
       <c r="D8" s="1">
-        <v>590097000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+        <v>611661000</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1984</v>
       </c>
       <c r="B9" s="1">
-        <v>1216860</v>
+        <v>1162220</v>
       </c>
       <c r="C9" s="1">
-        <v>688516</v>
+        <v>627459</v>
       </c>
       <c r="D9" s="1">
-        <v>815819000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+        <v>841932000</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1985</v>
       </c>
       <c r="B10" s="1">
-        <v>1254820</v>
+        <v>1212470</v>
       </c>
       <c r="C10" s="1">
-        <v>694819</v>
+        <v>639359</v>
       </c>
       <c r="D10" s="1">
-        <v>1193280000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+        <v>1237940000</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1986</v>
       </c>
       <c r="B11" s="1">
-        <v>1309800</v>
+        <v>1280810</v>
       </c>
       <c r="C11" s="1">
-        <v>702174</v>
+        <v>654070</v>
       </c>
       <c r="D11" s="1">
-        <v>1128640000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+        <v>1194520000</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1987</v>
       </c>
       <c r="B12" s="1">
-        <v>1375350</v>
+        <v>1359070</v>
       </c>
       <c r="C12" s="1">
-        <v>705764</v>
+        <v>665914</v>
       </c>
       <c r="D12" s="1">
-        <v>1085870000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+        <v>1130460000</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1988</v>
       </c>
       <c r="B13" s="1">
-        <v>1445950</v>
+        <v>1439900</v>
       </c>
       <c r="C13" s="1">
-        <v>703953</v>
+        <v>672254</v>
       </c>
       <c r="D13" s="1">
-        <v>1130780000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+        <v>1135930000</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1989</v>
       </c>
       <c r="B14" s="1">
-        <v>1516480</v>
+        <v>1518720</v>
       </c>
       <c r="C14" s="1">
-        <v>707453</v>
+        <v>683194</v>
       </c>
       <c r="D14" s="1">
-        <v>1043310000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+        <v>1052700000</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1990</v>
       </c>
       <c r="B15" s="1">
-        <v>1581460</v>
+        <v>1588960</v>
       </c>
       <c r="C15" s="1">
-        <v>728370</v>
+        <v>711093</v>
       </c>
       <c r="D15" s="1">
-        <v>910950000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+        <v>900815000</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1991</v>
       </c>
       <c r="B16" s="1">
-        <v>1634680</v>
+        <v>1647120</v>
       </c>
       <c r="C16" s="1">
-        <v>764725</v>
+        <v>755277</v>
       </c>
       <c r="D16" s="1">
-        <v>948296000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>965788000</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1992</v>
       </c>
       <c r="B17" s="1">
-        <v>1671040</v>
+        <v>1686450</v>
       </c>
       <c r="C17" s="1">
-        <v>806400</v>
+        <v>805153</v>
       </c>
       <c r="D17" s="1">
-        <v>944534000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>941991000</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1993</v>
       </c>
       <c r="B18" s="1">
-        <v>1686870</v>
+        <v>1704570</v>
       </c>
       <c r="C18" s="1">
-        <v>846735</v>
+        <v>852559</v>
       </c>
       <c r="D18" s="1">
-        <v>744599000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>755979000</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1994</v>
       </c>
       <c r="B19" s="1">
-        <v>1694130</v>
+        <v>1713670</v>
       </c>
       <c r="C19" s="1">
-        <v>886486</v>
+        <v>896927</v>
       </c>
       <c r="D19" s="1">
-        <v>734478000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>748876000</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1995</v>
       </c>
       <c r="B20" s="1">
-        <v>1690590</v>
+        <v>1711620</v>
       </c>
       <c r="C20" s="1">
-        <v>916642</v>
+        <v>929326</v>
       </c>
       <c r="D20" s="1">
-        <v>789498000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>804283000</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1996</v>
       </c>
       <c r="B21" s="1">
-        <v>1685320</v>
+        <v>1707530</v>
       </c>
       <c r="C21" s="1">
-        <v>941332</v>
+        <v>954797</v>
       </c>
       <c r="D21" s="1">
-        <v>768469000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>781478000</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1997</v>
       </c>
       <c r="B22" s="1">
-        <v>1679800</v>
+        <v>1703180</v>
       </c>
       <c r="C22" s="1">
-        <v>954485</v>
+        <v>968094</v>
       </c>
       <c r="D22" s="1">
-        <v>929790000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>948546000</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1998</v>
       </c>
       <c r="B23" s="1">
-        <v>1696960</v>
+        <v>1722050</v>
       </c>
       <c r="C23" s="1">
-        <v>965842</v>
+        <v>979539</v>
       </c>
       <c r="D23" s="1">
-        <v>1196990000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1223990000</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1999</v>
       </c>
       <c r="B24" s="1">
-        <v>1733510</v>
+        <v>1760430</v>
       </c>
       <c r="C24" s="1">
-        <v>970795</v>
+        <v>984532</v>
       </c>
       <c r="D24" s="1">
-        <v>1293470000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1317730000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2000</v>
       </c>
       <c r="B25" s="1">
-        <v>1797070</v>
+        <v>1825830</v>
       </c>
       <c r="C25" s="1">
-        <v>964397</v>
+        <v>978498</v>
       </c>
       <c r="D25" s="1">
-        <v>1653270000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1673490000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2001</v>
       </c>
       <c r="B26" s="1">
-        <v>1842760</v>
+        <v>1872940</v>
       </c>
       <c r="C26" s="1">
-        <v>948808</v>
+        <v>963368</v>
       </c>
       <c r="D26" s="1">
-        <v>1075310000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1090930000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2002</v>
       </c>
       <c r="B27" s="1">
-        <v>1884900</v>
+        <v>1915990</v>
       </c>
       <c r="C27" s="1">
-        <v>940853</v>
+        <v>955885</v>
       </c>
       <c r="D27" s="1">
-        <v>968251000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>980888000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2003</v>
       </c>
       <c r="B28" s="1">
-        <v>1912460</v>
+        <v>1944110</v>
       </c>
       <c r="C28" s="1">
-        <v>942759</v>
+        <v>958495</v>
       </c>
       <c r="D28" s="1">
-        <v>885333000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>898438000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2004</v>
       </c>
       <c r="B29" s="1">
-        <v>1921090</v>
+        <v>1953850</v>
       </c>
       <c r="C29" s="1">
-        <v>955425</v>
+        <v>972283</v>
       </c>
       <c r="D29" s="1">
-        <v>916966000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>945596000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2005</v>
       </c>
       <c r="B30" s="1">
-        <v>1938350</v>
+        <v>1971670</v>
       </c>
       <c r="C30" s="1">
-        <v>999117</v>
+        <v>1017170</v>
       </c>
       <c r="D30" s="1">
-        <v>950670000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>963776000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2006</v>
       </c>
       <c r="B31" s="1">
-        <v>1939990</v>
+        <v>1974060</v>
       </c>
       <c r="C31" s="1">
-        <v>1048390</v>
+        <v>1067450</v>
       </c>
       <c r="D31" s="1">
-        <v>880351000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>901356000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2007</v>
       </c>
       <c r="B32" s="1">
-        <v>1914480</v>
+        <v>1948590</v>
       </c>
       <c r="C32" s="1">
-        <v>1082140</v>
+        <v>1101730</v>
       </c>
       <c r="D32" s="1">
-        <v>649431000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>657857000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2008</v>
       </c>
       <c r="B33" s="1">
-        <v>1878300</v>
+        <v>1911700</v>
       </c>
       <c r="C33" s="1">
-        <v>1097230</v>
+        <v>1116820</v>
       </c>
       <c r="D33" s="1">
-        <v>624656000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>629211000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2009</v>
       </c>
       <c r="B34" s="1">
-        <v>1819940</v>
+        <v>1852080</v>
       </c>
       <c r="C34" s="1">
-        <v>1093150</v>
+        <v>1112700</v>
       </c>
       <c r="D34" s="1">
-        <v>468129000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>469784000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2010</v>
       </c>
       <c r="B35" s="1">
-        <v>1753930</v>
+        <v>1784290</v>
       </c>
       <c r="C35" s="1">
-        <v>1084960</v>
+        <v>1104620</v>
       </c>
       <c r="D35" s="1">
-        <v>457736000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>458856000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2011</v>
       </c>
       <c r="B36" s="1">
-        <v>1687170</v>
+        <v>1715490</v>
       </c>
       <c r="C36" s="1">
-        <v>1073700</v>
+        <v>1093620</v>
       </c>
       <c r="D36" s="1">
-        <v>584849000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>585089000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2012</v>
       </c>
       <c r="B37" s="1">
-        <v>1619140</v>
+        <v>1645110</v>
       </c>
       <c r="C37" s="1">
-        <v>1050800</v>
+        <v>1070520</v>
       </c>
       <c r="D37" s="1">
-        <v>689014000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>692029000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2013</v>
       </c>
       <c r="B38" s="1">
-        <v>1568030</v>
+        <v>1591340</v>
       </c>
       <c r="C38" s="1">
-        <v>1025530</v>
+        <v>1044590</v>
       </c>
       <c r="D38" s="1">
-        <v>700950000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>698914000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2014</v>
       </c>
       <c r="B39" s="1">
-        <v>1516180</v>
+        <v>1536590</v>
       </c>
       <c r="C39" s="1">
-        <v>987968</v>
+        <v>1005700</v>
       </c>
       <c r="D39" s="1">
-        <v>571774000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>569266000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2015</v>
       </c>
       <c r="B40" s="1">
-        <v>1449000</v>
+        <v>1466590</v>
       </c>
       <c r="C40" s="1">
-        <v>929376</v>
+        <v>945490</v>
       </c>
       <c r="D40" s="1">
-        <v>505884000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>502817000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2016</v>
       </c>
       <c r="B41" s="1">
-        <v>1404870</v>
+        <v>1419570</v>
       </c>
       <c r="C41" s="1">
-        <v>884077</v>
+        <v>898322</v>
       </c>
       <c r="D41" s="1">
-        <v>578368000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>573959000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2017</v>
       </c>
       <c r="B42" s="1">
-        <v>1366370</v>
+        <v>1378200</v>
       </c>
       <c r="C42" s="1">
-        <v>844001</v>
+        <v>856489</v>
       </c>
       <c r="D42" s="1">
-        <v>632992000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>625645000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2018</v>
       </c>
       <c r="B43" s="1">
-        <v>1338260</v>
+        <v>1347040</v>
       </c>
       <c r="C43" s="1">
-        <v>807968</v>
+        <v>818856</v>
       </c>
       <c r="D43" s="1">
-        <v>856700000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>844390000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2019</v>
       </c>
       <c r="B44" s="1">
-        <v>1315390</v>
+        <v>1321160</v>
       </c>
       <c r="C44" s="1">
-        <v>785828</v>
+        <v>795180</v>
       </c>
       <c r="D44" s="1">
-        <v>555772000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>544636000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2020</v>
       </c>
       <c r="B45" s="1">
-        <v>1293700</v>
+        <v>1296420</v>
       </c>
       <c r="C45" s="1">
-        <v>759757</v>
+        <v>767585</v>
       </c>
       <c r="D45" s="1">
-        <v>661233000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>648490000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2021</v>
       </c>
       <c r="B46" s="1">
-        <v>1279720</v>
+        <v>1279550</v>
       </c>
       <c r="C46" s="1">
-        <v>733359</v>
+        <v>739583</v>
       </c>
       <c r="D46" s="1">
-        <v>707335000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>697959000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2022</v>
       </c>
       <c r="B47" s="1">
-        <v>1281620</v>
+        <v>1278770</v>
       </c>
       <c r="C47" s="1">
-        <v>719298</v>
+        <v>723924</v>
       </c>
       <c r="D47" s="1">
-        <v>710551000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>699896000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2023</v>
       </c>
       <c r="B48" s="1">
-        <v>1270450</v>
+        <v>1265700</v>
       </c>
       <c r="C48" s="1">
-        <v>710935</v>
+        <v>713886</v>
       </c>
       <c r="D48" s="1">
         <v>436000000</v>
       </c>
+      <c r="E48" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>